<commit_message>
Preprocessamento - Organização dos dados iniciais
* Escolha dos parâmetros
* Formatação dos dados
* Binarização e one-hot encoding
</commit_message>
<xml_diff>
--- a/data/dicionario_de_dados.xlsx
+++ b/data/dicionario_de_dados.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\#ufrj_cursos_gravados\eel891_aprendizado_de_maquina\trabalhos\Trabalho1_Balanceado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Google Drive\Documentos\UFRJ\Períodos\7_2020.2\Aprendizado de Maquina\Trabalhos\T1-Sistema_apoio_decisao_aprovacao_credito\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEB0D33-63B1-4E8D-AE37-B46598AC66C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1B6165-4719-4101-B92A-64AD9118DE8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conjunto de Treinamento" sheetId="2" r:id="rId1"/>
     <sheet name="Conjunto de Teste" sheetId="3" r:id="rId2"/>
     <sheet name="Arquivo de Respostas" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Conjunto de Treinamento'!$A$1:$F$43</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="120">
   <si>
     <t>1,5,10,15,20,25</t>
   </si>
@@ -390,6 +382,9 @@
   </si>
   <si>
     <t>20001-25000</t>
+  </si>
+  <si>
+    <t>Relevante</t>
   </si>
 </sst>
 </file>
@@ -861,7 +856,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -871,6 +866,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="40">
@@ -1249,516 +1247,616 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="94" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="94" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
+      <c r="B4" s="4">
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1766,30 +1864,36 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1797,16 +1901,19 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1814,16 +1921,19 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1831,16 +1941,19 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1848,16 +1961,19 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1865,16 +1981,19 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1882,13 +2001,16 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1896,13 +2018,16 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1910,19 +2035,28 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F43" xr:uid="{6DA35FF1-6386-4BB4-B75C-F79E289F6ECB}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>